<commit_message>
Add pandas full docs with new getting started
</commit_message>
<xml_diff>
--- a/pandas-docs/source/user_guide/styled.xlsx
+++ b/pandas-docs/source/user_guide/styled.xlsx
@@ -1,36 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-</sst>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,23 +26,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color rgb="00FF0000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
@@ -94,22 +65,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -408,26 +378,36 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -437,7 +417,7 @@
       <c r="C2" s="2" t="n">
         <v>1.329212172649186</v>
       </c>
-      <c r="D2" s="2" t="s"/>
+      <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="3" t="n">
         <v>-0.3162803596214298</v>
       </c>
@@ -445,7 +425,7 @@
         <v>-0.990810386640961</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -465,7 +445,7 @@
         <v>0.2957218876223381</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -485,7 +465,7 @@
         <v>1.889272731415282</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -498,14 +478,12 @@
       <c r="D5" s="2" t="n">
         <v>0.1040111956837392</v>
       </c>
-      <c r="E5" s="3" t="n">
-        <v>-0.481165317281003</v>
-      </c>
+      <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="n">
         <v>0.8502285312282443</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -525,7 +503,7 @@
         <v>0.515018378039662</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -545,7 +523,7 @@
         <v>-0.06332798345060607</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -565,7 +543,7 @@
         <v>1.627795744482153</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
@@ -585,7 +563,7 @@
         <v>0.5198180007843201</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -605,7 +583,7 @@
         <v>-2.089354277469368</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
@@ -626,6 +604,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>